<commit_message>
jadwal pelaksanaan, surat keterangan, nilai, link untuk pas foto dan ktmktp pada excel
</commit_message>
<xml_diff>
--- a/public/template/jadwal_pelaksanaan_template.xlsx
+++ b/public/template/jadwal_pelaksanaan_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\toeic\file_import_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\toeic\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A47143-894C-41F0-8EAC-C857E1EFA979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD47B13-3B3B-4C8C-A9F9-8B4C3200654A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{CCCC91B2-35A4-433D-B4D1-963FC7824957}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>NIM</t>
   </si>
@@ -46,16 +46,38 @@
   </si>
   <si>
     <t>25-8-2025</t>
+  </si>
+  <si>
+    <t>link zoom</t>
+  </si>
+  <si>
+    <t>https://us05web.zoom.us/j/83990720254?pwd=2BJciSFGDWGEaP2QzQILctCFu0D4Hv.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,15 +100,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipertaut" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A382D5E1-BB7E-4E8F-AB50-0AE0DFAC35D2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,20 +436,24 @@
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="65" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2341760196</v>
       </c>
@@ -433,8 +463,11 @@
       <c r="C2" s="2">
         <v>0.375</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2341760036</v>
       </c>
@@ -444,8 +477,15 @@
       <c r="C3" s="2">
         <v>0.33333333333333331</v>
       </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{C6E92534-D586-4226-9564-DBE8B64FF85B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>